<commit_message>
Lab 5 -  Completed upto Q4 Project -  Handled services not in list
</commit_message>
<xml_diff>
--- a/Final Project/Service_details.xlsx
+++ b/Final Project/Service_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Chathuranga/Desktop/Masters Lecture Docs/Text Mining 732A92 /Labs/Text Mining Labs/Final Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D643AA-4883-5648-98D7-4F747FBC96B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A693BCE7-E527-A341-B97B-8A54C5C65EB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9480" yWindow="460" windowWidth="24640" windowHeight="13320" xr2:uid="{90BCE67B-5652-B640-AD52-7EDC21B123A1}"/>
+    <workbookView xWindow="1260" yWindow="1760" windowWidth="24640" windowHeight="13320" xr2:uid="{90BCE67B-5652-B640-AD52-7EDC21B123A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>Code</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>ERROR</t>
+  </si>
+  <si>
+    <t>Sorry I'm not aware about this service. Hence I will inform this to the management and will reach back to you.</t>
+  </si>
+  <si>
+    <t>G000</t>
+  </si>
+  <si>
+    <t>This is Info about saloon services in general!</t>
   </si>
 </sst>
 </file>
@@ -424,16 +436,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF738C3-469E-AA4E-BCA7-D59436515668}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="1" customWidth="1"/>
-    <col min="2" max="2" width="81.6640625" customWidth="1"/>
+    <col min="2" max="2" width="152.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -446,15 +458,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -462,15 +474,15 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -478,7 +490,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -486,7 +498,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -494,7 +506,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -502,10 +514,26 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed Up to - Results section on report
</commit_message>
<xml_diff>
--- a/Final Project/Service_details.xlsx
+++ b/Final Project/Service_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Chathuranga/Desktop/Masters Lecture Docs/Text Mining 732A92 /Labs/Text Mining Labs/Final Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF2D8C9-11A6-7E48-A94A-AF86893321DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68E9021-81F7-1348-A2C1-C85F17759161}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="1560" windowWidth="24640" windowHeight="13320" xr2:uid="{90BCE67B-5652-B640-AD52-7EDC21B123A1}"/>
+    <workbookView xWindow="2560" yWindow="460" windowWidth="24640" windowHeight="13320" xr2:uid="{90BCE67B-5652-B640-AD52-7EDC21B123A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Code</t>
   </si>
@@ -69,9 +69,6 @@
     <t>We are providing Hair cuts for Ladies, Gents and Children hair cuts. Ladies Hair cut 20$ upwards. Gents Hair cut 10$ upwards. And we have special children hair cuts 6$ upwards.</t>
   </si>
   <si>
-    <t>Pass</t>
-  </si>
-  <si>
     <t>ERROR</t>
   </si>
   <si>
@@ -81,7 +78,47 @@
     <t>G000</t>
   </si>
   <si>
-    <t>This is Info about saloon services in general!</t>
+    <t>G001-1</t>
+  </si>
+  <si>
+    <t>Haircut for those a little younger. Applies to children up to 10 years. From $ 15</t>
+  </si>
+  <si>
+    <t>G001-2</t>
+  </si>
+  <si>
+    <t>We have special haircut styles for Men. From $ 20</t>
+  </si>
+  <si>
+    <t>G001-3</t>
+  </si>
+  <si>
+    <t>We have special haircut styles for Womens. From $ 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We give you current hairstyle tips and treatments around ongoing hair trends, always with professional hair care products. We provide Hair cutting, Coloring, Dressing, Steups, Hair massages, Facials, Predicure and Manicures. Our prices are based on our experience and on time and material needs, and are from-prices. Exact price can be given after consultation with your hairdresser. We are a cashless salon, we take debit / credit cards. By the way you could make appointments through chat :) </t>
+  </si>
+  <si>
+    <t>We have hair dressings with complementry facials. From $ 30</t>
+  </si>
+  <si>
+    <t>We provide hair setups with complementry face massage. From $ 30</t>
+  </si>
+  <si>
+    <t>30 luxurious minutes with care for your hair and scalp. A special treatment. Long durability that takes care of your hair. From $ 35</t>
+  </si>
+  <si>
+    <t>We will take care all of you face skin treatments and makeups with quality prodcuts in the industry. From $ 40</t>
+  </si>
+  <si>
+    <t>Kick up your heels and enjoy a spa staple with a pedicure. Your feet will be polished and massaged to pretty perfection, and you’ll leave a more relaxed and more comfortable person. During a spa pedicure you should expect your feet to be soaked in warm water and your nails to be cut and shaped. Your nail spa therapist will use a pumice stone to buff away dry skin, and will follow up with an exfoliation. Prices from $ 50</t>
+  </si>
+  <si>
+    <t>With nail salon services ranging from gel, acrylics, paraffin dips, and nail art, there is something for everyone looking for a manicure. Whether you just want a basic grooming and polish or want to go all out with 3D art and gradients. They help ensure healthy nails and hands and are a quick and easy way to change or polish your look. Prices from $ 20</t>
+  </si>
+  <si>
+    <t>Simple coloring or alternatively loops (not foil loops). Haircuts and lighter styling are included. NOTE! All prices are from-prices, exact price can be given after consultation with your hairdresser.
+In some cases, decolorization / deep cleaning may be needed before other treatment. Have you dyed your hair before or done any other type of color treatment? Contact the salon before booking.</t>
   </si>
 </sst>
 </file>
@@ -117,10 +154,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -436,104 +476,128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF738C3-469E-AA4E-BCA7-D59436515668}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11" style="1" customWidth="1"/>
-    <col min="2" max="2" width="152.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11" style="2" customWidth="1"/>
+    <col min="2" max="2" width="91.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:2" ht="62" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="B14" t="s">
         <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>